<commit_message>
fixed column charge and merged file
</commit_message>
<xml_diff>
--- a/impact_analysis/data/impact_analysis_config_new.xlsx
+++ b/impact_analysis/data/impact_analysis_config_new.xlsx
@@ -48,7 +48,7 @@
     <t>Start</t>
   </si>
   <si>
-    <t>impact_analysis/data/input/file1.xlsx</t>
+    <t>data/input/file1.xlsx</t>
   </si>
   <si>
     <t>PREMIUM_AMOUNT_Property</t>
@@ -57,13 +57,13 @@
     <t xml:space="preserve">Excess Change</t>
   </si>
   <si>
-    <t>impact_analysis/data/input/file2.xlsx</t>
+    <t>data/input/file2.xlsx</t>
   </si>
   <si>
     <t>Inflation</t>
   </si>
   <si>
-    <t>impact_analysis/data/input/file3.xlsx</t>
+    <t>data/input/file3.xlsx</t>
   </si>
   <si>
     <t>BI</t>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="top"/>
@@ -153,8 +153,9 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" quotePrefix="0" pivotButton="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +743,7 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
@@ -762,10 +763,10 @@
       <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -782,7 +783,7 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
@@ -802,10 +803,10 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -825,7 +826,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -857,7 +858,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -886,13 +887,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>